<commit_message>
Full export of brewery as built in world
</commit_message>
<xml_diff>
--- a/Brewery Coordinates and Prim Counts.xlsx
+++ b/Brewery Coordinates and Prim Counts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="30">
   <si>
     <t>Building</t>
   </si>
@@ -73,6 +73,39 @@
   </si>
   <si>
     <t>House</t>
+  </si>
+  <si>
+    <t>What are you drinking</t>
+  </si>
+  <si>
+    <t>Export</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>(mega prims)</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>(some textures fail)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>(too hard to get too)</t>
+  </si>
+  <si>
+    <t>permissions!</t>
+  </si>
+  <si>
+    <t>textures</t>
+  </si>
+  <si>
+    <t>copy of other</t>
   </si>
 </sst>
 </file>
@@ -404,15 +437,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E16"/>
+      <selection activeCell="E2" sqref="E2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -425,8 +458,11 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5">
+      <c r="F1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -442,8 +478,14 @@
       <c r="E2">
         <v>15</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="F2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -459,16 +501,28 @@
       <c r="E3">
         <v>20</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="F3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="F4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -484,8 +538,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="F5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -501,8 +558,14 @@
       <c r="E6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5">
+      <c r="F6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -518,8 +581,11 @@
       <c r="E7">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5">
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -535,8 +601,14 @@
       <c r="E8">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:5">
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -552,8 +624,11 @@
       <c r="E9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:5">
+      <c r="F9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -569,53 +644,106 @@
       <c r="E10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5">
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="E11">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5">
+      <c r="F11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12" t="s">
         <v>14</v>
       </c>
       <c r="E12">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5">
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
       <c r="A13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13" t="e">
+        <f>NA()</f>
+        <v>#N/A</v>
+      </c>
+      <c r="G13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" t="s">
         <v>15</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:5">
-      <c r="A14" t="s">
+      <c r="F14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" t="s">
         <v>16</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5">
-      <c r="A15" t="s">
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
         <v>17</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5">
-      <c r="A16" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
         <v>18</v>
       </c>
-      <c r="E16">
-        <v>1</v>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v1.1 Changes ready to merge to trunk
</commit_message>
<xml_diff>
--- a/Brewery Coordinates and Prim Counts.xlsx
+++ b/Brewery Coordinates and Prim Counts.xlsx
@@ -440,7 +440,7 @@
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E18"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -470,7 +470,7 @@
         <v>128.09200000000001</v>
       </c>
       <c r="C2">
-        <v>39.939</v>
+        <v>39.914999999999999</v>
       </c>
       <c r="D2">
         <v>152.86500000000001</v>

</xml_diff>

<commit_message>
Prim count updates New InfoHub script
</commit_message>
<xml_diff>
--- a/Brewery Coordinates and Prim Counts.xlsx
+++ b/Brewery Coordinates and Prim Counts.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t>Building</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Static?</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Wardrobe</t>
   </si>
   <si>
@@ -136,6 +133,15 @@
   </si>
   <si>
     <t>but you'll fall ??</t>
+  </si>
+  <si>
+    <t>Now part of brewery</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Potential freed =</t>
   </si>
 </sst>
 </file>
@@ -467,18 +473,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:11">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -497,8 +505,15 @@
       <c r="H1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1">
+        <f>SUM(J:J)-COUNT(J:J)</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,8 +538,11 @@
       <c r="H2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="J2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -550,7 +568,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:11">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -567,7 +585,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:11">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -586,11 +604,17 @@
       <c r="F5" t="s">
         <v>2</v>
       </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
       <c r="H5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="J5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -615,8 +639,11 @@
       <c r="H6" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -635,11 +662,17 @@
       <c r="F7" t="s">
         <v>2</v>
       </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
       <c r="H7" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
+        <v>40</v>
+      </c>
+      <c r="J7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -664,8 +697,11 @@
       <c r="H8" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -687,8 +723,11 @@
       <c r="H9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -711,7 +750,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="11" spans="1:8">
+    <row r="11" spans="1:11">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -728,7 +767,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:11">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -742,7 +781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:11">
       <c r="A13" t="s">
         <v>14</v>
       </c>
@@ -760,7 +799,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:11">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -771,13 +810,13 @@
         <v>2</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H14" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:11">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -794,7 +833,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:11">
       <c r="A16" t="s">
         <v>17</v>
       </c>
@@ -808,7 +847,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="1:9">
+    <row r="17" spans="1:10">
       <c r="A17" t="s">
         <v>18</v>
       </c>
@@ -819,10 +858,10 @@
         <v>2</v>
       </c>
       <c r="I17" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18" t="s">
         <v>19</v>
       </c>
@@ -839,9 +878,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:9">
+    <row r="19" spans="1:10">
       <c r="A19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E19">
         <v>8</v>
@@ -853,9 +892,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="20" spans="1:9">
+    <row r="20" spans="1:10">
       <c r="A20" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E20">
         <v>8</v>
@@ -867,12 +906,12 @@
         <v>23</v>
       </c>
       <c r="I20" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E21">
         <v>20</v>
@@ -881,15 +920,18 @@
         <v>21</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="H21" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:9">
+      <c r="J21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E22">
         <v>4</v>
@@ -899,6 +941,9 @@
       </c>
       <c r="H22" t="s">
         <v>2</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>